<commit_message>
Decile scaling to improve contrast
</commit_message>
<xml_diff>
--- a/weather_data.xlsx
+++ b/weather_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clare\Documents\Clare\2017-2018\INFO_3300\Project 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelzhang/Documents/GitHub/CS-3300-P2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C3ECC6-FE78-454F-8C99-3F468FB712C5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11460" windowHeight="6563"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weather_data" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="15">
   <si>
     <t>Winter</t>
   </si>
@@ -61,11 +62,25 @@
   <si>
     <t>Napa</t>
   </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Decile</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="3">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="172" formatCode="0.00000000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,12 +110,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,7 +151,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -442,19 +463,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F161"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J153" sqref="J153"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="6" width="9.06640625" style="2"/>
+    <col min="4" max="6" width="9" style="2"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -473,8 +497,20 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="J1" s="2" t="str">
+        <f>D1</f>
+        <v>precip_day</v>
+      </c>
+      <c r="K1" s="2" t="str">
+        <f>E1</f>
+        <v>precip_avg</v>
+      </c>
+      <c r="L1" s="2" t="str">
+        <f>F1</f>
+        <v>temp_avg</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -493,8 +529,23 @@
       <c r="F2" s="2">
         <v>51.033333333333331</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2">
+        <f>MIN(D2:D161)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <f>MIN(E2:E161)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <f>MIN(F2:F161)</f>
+        <v>45.349999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -513,8 +564,26 @@
       <c r="F3" s="2">
         <v>58.766666666666673</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3">
+        <f>PERCENTILE(D$2:D$161,0.1)</f>
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <f>PERCENTILE(E$2:E$161,0.1)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <f>PERCENTILE(F$2:F$161,0.1)</f>
+        <v>48.323333333333338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -533,8 +602,24 @@
       <c r="F4" s="2">
         <v>68.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H4" s="5"/>
+      <c r="I4" s="2">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3">
+        <f>PERCENTILE($D$2:$D$161,0.2)</f>
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f>PERCENTILE(E$2:E$161,0.2)</f>
+        <v>4.4666666666666612E-2</v>
+      </c>
+      <c r="L4" s="6">
+        <f>PERCENTILE(F$2:F$161,0.2)</f>
+        <v>50.033333333333331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -553,8 +638,24 @@
       <c r="F5" s="2">
         <v>61.533333333333331</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H5" s="5"/>
+      <c r="I5" s="2">
+        <v>30</v>
+      </c>
+      <c r="J5" s="3">
+        <f>PERCENTILE($D$2:$D$161,0.3)</f>
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <f>PERCENTILE(E$2:E$161,0.3)</f>
+        <v>0.18203333333333332</v>
+      </c>
+      <c r="L5" s="6">
+        <f>PERCENTILE(F$2:F$161,0.3)</f>
+        <v>54.609999999999992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -573,8 +674,24 @@
       <c r="F6" s="2">
         <v>49.733333333333327</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H6" s="5"/>
+      <c r="I6" s="2">
+        <v>40</v>
+      </c>
+      <c r="J6" s="3">
+        <f>PERCENTILE($D$2:$D$161,0.4)</f>
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <f>PERCENTILE(E$2:E$161,0.4)</f>
+        <v>0.25062279386811614</v>
+      </c>
+      <c r="L6" s="6">
+        <f>PERCENTILE(F$2:F$161,0.4)</f>
+        <v>57.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -593,8 +710,24 @@
       <c r="F7" s="2">
         <v>60.966666666666661</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H7" s="5"/>
+      <c r="I7" s="2">
+        <v>50</v>
+      </c>
+      <c r="J7" s="3">
+        <f>PERCENTILE($D$2:$D$161,0.5)</f>
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <f>PERCENTILE(E$2:E$161,0.5)</f>
+        <v>0.31125000000000003</v>
+      </c>
+      <c r="L7" s="6">
+        <f>PERCENTILE(F$2:F$161,0.5)</f>
+        <v>59.774999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -613,8 +746,24 @@
       <c r="F8" s="2">
         <v>69.900000000000006</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H8" s="5"/>
+      <c r="I8" s="2">
+        <v>60</v>
+      </c>
+      <c r="J8" s="3">
+        <f>PERCENTILE($D$2:$D$161,0.6)</f>
+        <v>13</v>
+      </c>
+      <c r="K8">
+        <f>PERCENTILE(E$2:E$161,0.6)</f>
+        <v>0.35900432900432899</v>
+      </c>
+      <c r="L8" s="6">
+        <f>PERCENTILE(F$2:F$161,0.6)</f>
+        <v>61.586666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -633,8 +782,24 @@
       <c r="F9" s="2">
         <v>52.566666666666663</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H9" s="5"/>
+      <c r="I9" s="2">
+        <v>70</v>
+      </c>
+      <c r="J9" s="3">
+        <f>PERCENTILE($D$2:$D$161,0.7)</f>
+        <v>17</v>
+      </c>
+      <c r="K9">
+        <f>PERCENTILE(E$2:E$161,0.7)</f>
+        <v>0.42491666666666666</v>
+      </c>
+      <c r="L9" s="6">
+        <f>PERCENTILE(F$2:F$161,0.7)</f>
+        <v>63.339999999999989</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -653,8 +818,24 @@
       <c r="F10" s="2">
         <v>48.333333333333336</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H10" s="5"/>
+      <c r="I10" s="2">
+        <v>80</v>
+      </c>
+      <c r="J10" s="3">
+        <f>PERCENTILE($D$2:$D$161,0.8)</f>
+        <v>22</v>
+      </c>
+      <c r="K10">
+        <f>PERCENTILE(E$2:E$161,0.8)</f>
+        <v>0.47893333333333327</v>
+      </c>
+      <c r="L10" s="6">
+        <f>PERCENTILE(F$2:F$161,0.8)</f>
+        <v>68.444000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -673,8 +854,24 @@
       <c r="F11" s="2">
         <v>56.15</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H11" s="5"/>
+      <c r="I11" s="2">
+        <v>90</v>
+      </c>
+      <c r="J11" s="3">
+        <f>PERCENTILE($D$2:$D$161,0.9)</f>
+        <v>30.099999999999994</v>
+      </c>
+      <c r="K11">
+        <f>PERCENTILE(E$2:E$161,0.9)</f>
+        <v>0.58438333333333325</v>
+      </c>
+      <c r="L11" s="6">
+        <f>PERCENTILE(F$2:F$161,0.9)</f>
+        <v>72.98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -693,8 +890,24 @@
       <c r="F12" s="2">
         <v>70.099999999999994</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H12" s="5"/>
+      <c r="I12" s="2">
+        <v>100</v>
+      </c>
+      <c r="J12" s="3">
+        <f>PERCENTILE($D$2:$D$161,1)</f>
+        <v>53</v>
+      </c>
+      <c r="K12">
+        <f>PERCENTILE(E$2:E$161,1)</f>
+        <v>1.0184444444444445</v>
+      </c>
+      <c r="L12" s="6">
+        <f>PERCENTILE(F$2:F$161,1)</f>
+        <v>76.13333333333334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -713,8 +926,23 @@
       <c r="F13" s="2">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="2">
+        <f>MAX(D2:D161)</f>
+        <v>53</v>
+      </c>
+      <c r="K13" s="4">
+        <f>MAX(E2:E161)</f>
+        <v>1.0184444444444445</v>
+      </c>
+      <c r="L13" s="6">
+        <f>MAX(F2:F161)</f>
+        <v>76.13333333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -734,7 +962,7 @@
         <v>48.066666666666663</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -754,7 +982,7 @@
         <v>53.650000000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -774,7 +1002,7 @@
         <v>66.2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -794,7 +1022,7 @@
         <v>55.2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -814,7 +1042,7 @@
         <v>49.9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -834,7 +1062,7 @@
         <v>58.9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -854,7 +1082,7 @@
         <v>73.400000000000006</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -874,7 +1102,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -894,7 +1122,7 @@
         <v>48.133333333333326</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -914,7 +1142,7 @@
         <v>59.699999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -934,7 +1162,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -954,7 +1182,7 @@
         <v>61.199999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -974,7 +1202,7 @@
         <v>49.266666666666673</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -994,7 +1222,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1014,7 +1242,7 @@
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1034,7 +1262,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1054,7 +1282,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1074,7 +1302,7 @@
         <v>53.55</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1094,7 +1322,7 @@
         <v>68.099999999999994</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1114,7 +1342,7 @@
         <v>60.4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1134,7 +1362,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1154,7 +1382,7 @@
         <v>60.466666666666669</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1174,7 +1402,7 @@
         <v>69.699999999999989</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1194,7 +1422,7 @@
         <v>61.366666666666667</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1214,7 +1442,7 @@
         <v>49.633333333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1234,7 +1462,7 @@
         <v>58.1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1254,7 +1482,7 @@
         <v>64.2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1274,7 +1502,7 @@
         <v>59.85</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1294,7 +1522,7 @@
         <v>49.033333333333331</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -1314,7 +1542,7 @@
         <v>55.45</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -1334,7 +1562,7 @@
         <v>62.6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -1354,7 +1582,7 @@
         <v>53.4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1374,7 +1602,7 @@
         <v>47.333333333333336</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -1394,7 +1622,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -1414,7 +1642,7 @@
         <v>69.300000000000011</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -1434,7 +1662,7 @@
         <v>57.31</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -1454,7 +1682,7 @@
         <v>46.966666666666669</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -1474,7 +1702,7 @@
         <v>57.633333333333333</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -1494,7 +1722,7 @@
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -1514,7 +1742,7 @@
         <v>55.7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -1534,7 +1762,7 @@
         <v>47.349999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -1554,7 +1782,7 @@
         <v>57.033333333333331</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -1574,7 +1802,7 @@
         <v>66.349999999999994</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -1594,7 +1822,7 @@
         <v>52.4</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -1614,7 +1842,7 @@
         <v>49.7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -1634,7 +1862,7 @@
         <v>58.3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -1654,7 +1882,7 @@
         <v>68.430000000000007</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -1674,7 +1902,7 @@
         <v>53.3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -1694,7 +1922,7 @@
         <v>49.8</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -1714,7 +1942,7 @@
         <v>53.95</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -1734,7 +1962,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -1754,7 +1982,7 @@
         <v>56.2</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -1774,7 +2002,7 @@
         <v>49.3</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -1794,7 +2022,7 @@
         <v>58.14</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -1814,7 +2042,7 @@
         <v>69.23</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -1834,7 +2062,7 @@
         <v>60.766666666666673</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -1854,7 +2082,7 @@
         <v>45.349999999999994</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -1874,7 +2102,7 @@
         <v>59.233333333333327</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -1894,7 +2122,7 @@
         <v>68.333333333333329</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -1914,7 +2142,7 @@
         <v>63.550000000000004</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -1934,7 +2162,7 @@
         <v>52.066666666666663</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -1954,7 +2182,7 @@
         <v>56.156097560975589</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -1974,7 +2202,7 @@
         <v>68.966666666666654</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -1994,7 +2222,7 @@
         <v>63.133333333333333</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -2014,7 +2242,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -2034,7 +2262,7 @@
         <v>58.266666666666673</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -2054,7 +2282,7 @@
         <v>70.36666666666666</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -2074,7 +2302,7 @@
         <v>62.433333333333337</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -2094,7 +2322,7 @@
         <v>50.066666666666663</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -2114,7 +2342,7 @@
         <v>58.333333333333336</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -2134,7 +2362,7 @@
         <v>75.7</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -2154,7 +2382,7 @@
         <v>62.566666666666663</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>11</v>
       </c>
@@ -2174,7 +2402,7 @@
         <v>47.55</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -2194,7 +2422,7 @@
         <v>61.933333333333302</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -2214,7 +2442,7 @@
         <v>74.033333333333331</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -2234,7 +2462,7 @@
         <v>63.29999999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -2254,7 +2482,7 @@
         <v>47.033333333333331</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -2274,7 +2502,7 @@
         <v>54.699999999999996</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -2294,7 +2522,7 @@
         <v>72.833333333333329</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>11</v>
       </c>
@@ -2314,7 +2542,7 @@
         <v>61.966666666666669</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>11</v>
       </c>
@@ -2334,7 +2562,7 @@
         <v>46.866666666666667</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>11</v>
       </c>
@@ -2354,7 +2582,7 @@
         <v>56.366666666666667</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -2374,7 +2602,7 @@
         <v>72.3</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -2394,7 +2622,7 @@
         <v>64.333333333333329</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -2414,7 +2642,7 @@
         <v>48.533333333333331</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -2434,7 +2662,7 @@
         <v>59.366666666666667</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -2454,7 +2682,7 @@
         <v>73.63333333333334</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -2474,7 +2702,7 @@
         <v>60.4</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -2494,7 +2722,7 @@
         <v>46.633333333333326</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -2514,7 +2742,7 @@
         <v>60.766666666666659</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -2534,7 +2762,7 @@
         <v>74.733333333333334</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>11</v>
       </c>
@@ -2554,7 +2782,7 @@
         <v>64.566666666666663</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -2574,7 +2802,7 @@
         <v>48.233333333333327</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>11</v>
       </c>
@@ -2594,7 +2822,7 @@
         <v>57.833333333333336</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>11</v>
       </c>
@@ -2614,7 +2842,7 @@
         <v>74.766666666666666</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -2634,7 +2862,7 @@
         <v>63.43333333333333</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -2654,7 +2882,7 @@
         <v>49.6</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -2674,7 +2902,7 @@
         <v>57.6</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>11</v>
       </c>
@@ -2694,7 +2922,7 @@
         <v>76.13333333333334</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>11</v>
       </c>
@@ -2714,7 +2942,7 @@
         <v>64.866666666666674</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>11</v>
       </c>
@@ -2734,7 +2962,7 @@
         <v>48.333333333333336</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -2754,7 +2982,7 @@
         <v>61.800000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>11</v>
       </c>
@@ -2774,7 +3002,7 @@
         <v>74.86666666666666</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -2794,7 +3022,7 @@
         <v>62.666666666666664</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>11</v>
       </c>
@@ -2814,7 +3042,7 @@
         <v>48.966666666666661</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>11</v>
       </c>
@@ -2834,7 +3062,7 @@
         <v>58.533333333333331</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>11</v>
       </c>
@@ -2854,7 +3082,7 @@
         <v>74.899999999999991</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -2874,7 +3102,7 @@
         <v>62.666666666666664</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>11</v>
       </c>
@@ -2894,7 +3122,7 @@
         <v>48.800000000000004</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -2914,7 +3142,7 @@
         <v>56.533333333333331</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>11</v>
       </c>
@@ -2934,7 +3162,7 @@
         <v>75.333333333333329</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>11</v>
       </c>
@@ -2954,7 +3182,7 @@
         <v>61.933333333333337</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>11</v>
       </c>
@@ -2974,7 +3202,7 @@
         <v>46.966666666666661</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>11</v>
       </c>
@@ -2994,7 +3222,7 @@
         <v>60.133333333333333</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>11</v>
       </c>
@@ -3014,7 +3242,7 @@
         <v>72.899999999999991</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>11</v>
       </c>
@@ -3034,7 +3262,7 @@
         <v>61.666666666666664</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>11</v>
       </c>
@@ -3054,7 +3282,7 @@
         <v>46.166666666666664</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>11</v>
       </c>
@@ -3074,7 +3302,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>11</v>
       </c>
@@ -3094,7 +3322,7 @@
         <v>75.133333333333326</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>11</v>
       </c>
@@ -3114,7 +3342,7 @@
         <v>64.166666666666671</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>11</v>
       </c>
@@ -3134,7 +3362,7 @@
         <v>47.366666666666667</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>11</v>
       </c>
@@ -3154,7 +3382,7 @@
         <v>61.4</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>11</v>
       </c>
@@ -3174,7 +3402,7 @@
         <v>73.63333333333334</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>11</v>
       </c>
@@ -3194,7 +3422,7 @@
         <v>63.266666666666673</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>11</v>
       </c>
@@ -3214,7 +3442,7 @@
         <v>49.433333333333337</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>11</v>
       </c>
@@ -3234,7 +3462,7 @@
         <v>54.4</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>11</v>
       </c>
@@ -3254,7 +3482,7 @@
         <v>72.933333333333337</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -3274,7 +3502,7 @@
         <v>62.9</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>11</v>
       </c>
@@ -3294,7 +3522,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -3314,7 +3542,7 @@
         <v>55.366666666666667</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>11</v>
       </c>
@@ -3334,7 +3562,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>11</v>
       </c>
@@ -3354,7 +3582,7 @@
         <v>62.9</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>11</v>
       </c>
@@ -3374,7 +3602,7 @@
         <v>48.666666666666664</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>11</v>
       </c>
@@ -3394,7 +3622,7 @@
         <v>57.666666666666664</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>11</v>
       </c>
@@ -3414,7 +3642,7 @@
         <v>74.033333333333331</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -3434,7 +3662,7 @@
         <v>64.133333333333326</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>11</v>
       </c>
@@ -3454,7 +3682,7 @@
         <v>46.366666666666674</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -3474,7 +3702,7 @@
         <v>60.70000000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>11</v>
       </c>
@@ -3494,7 +3722,7 @@
         <v>74.666666666666657</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>11</v>
       </c>
@@ -3514,7 +3742,7 @@
         <v>62.29999999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>11</v>
       </c>
@@ -3534,7 +3762,7 @@
         <v>51.800000000000004</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>11</v>
       </c>
@@ -3554,7 +3782,7 @@
         <v>61.066666666666663</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>11</v>
       </c>
@@ -3574,7 +3802,7 @@
         <v>75.666666666666671</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>11</v>
       </c>
@@ -3594,7 +3822,7 @@
         <v>64.433333333333337</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>11</v>
       </c>
@@ -3614,7 +3842,7 @@
         <v>50.666666666666664</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>11</v>
       </c>
@@ -3634,7 +3862,7 @@
         <v>60.466666666666669</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>11</v>
       </c>
@@ -3654,7 +3882,7 @@
         <v>75.466666666666654</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>11</v>
       </c>
@@ -3675,6 +3903,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H3:H12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>